<commit_message>
files on city Officials during covid
</commit_message>
<xml_diff>
--- a/CN_Provinces/CN_Policy/V3-Yuhang_Pan-CN_lockdown_data.xlsx
+++ b/CN_Provinces/CN_Policy/V3-Yuhang_Pan-CN_lockdown_data.xlsx
@@ -1105,7 +1105,7 @@
         <v>43854</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1140,7 +1140,7 @@
         <v>43855</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1245,7 +1245,7 @@
         <v>43855</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1385,7 +1385,7 @@
         <v>43855</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1455,7 +1455,7 @@
         <v>43862</v>
       </c>
       <c r="K12">
-        <v>7</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1490,7 +1490,7 @@
         <v>43855</v>
       </c>
       <c r="K13">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1525,7 +1525,7 @@
         <v>43854</v>
       </c>
       <c r="K14">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1560,7 +1560,7 @@
         <v>43854</v>
       </c>
       <c r="K15">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1630,7 +1630,7 @@
         <v>43876</v>
       </c>
       <c r="K17">
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1665,7 +1665,7 @@
         <v>43854</v>
       </c>
       <c r="K18">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1700,7 +1700,7 @@
         <v>43854</v>
       </c>
       <c r="K19">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1735,7 +1735,7 @@
         <v>43858</v>
       </c>
       <c r="K20">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1770,7 +1770,7 @@
         <v>43854</v>
       </c>
       <c r="K21">
-        <v>-9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1805,7 +1805,7 @@
         <v>43854</v>
       </c>
       <c r="K22">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1840,7 +1840,7 @@
         <v>43854</v>
       </c>
       <c r="K23">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1875,7 +1875,7 @@
         <v>43854</v>
       </c>
       <c r="K24">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1910,7 +1910,7 @@
         <v>43854</v>
       </c>
       <c r="K25">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1945,7 +1945,7 @@
         <v>43857</v>
       </c>
       <c r="K26">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1980,7 +1980,7 @@
         <v>43855</v>
       </c>
       <c r="K27">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2015,7 +2015,7 @@
         <v>43854</v>
       </c>
       <c r="K28">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2050,7 +2050,7 @@
         <v>43854</v>
       </c>
       <c r="K29">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2085,7 +2085,7 @@
         <v>43854</v>
       </c>
       <c r="K30">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2120,7 +2120,7 @@
         <v>43854</v>
       </c>
       <c r="K31">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2155,7 +2155,7 @@
         <v>43855</v>
       </c>
       <c r="K32">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2190,7 +2190,7 @@
         <v>43857</v>
       </c>
       <c r="K33">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2225,7 +2225,7 @@
         <v>43854</v>
       </c>
       <c r="K34">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2260,7 +2260,7 @@
         <v>43854</v>
       </c>
       <c r="K35">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2295,7 +2295,7 @@
         <v>43855</v>
       </c>
       <c r="K36">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2330,7 +2330,7 @@
         <v>43854</v>
       </c>
       <c r="K37">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2365,7 +2365,7 @@
         <v>43854</v>
       </c>
       <c r="K38">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2400,7 +2400,7 @@
         <v>43862</v>
       </c>
       <c r="K39">
-        <v>-4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2435,7 +2435,7 @@
         <v>43876</v>
       </c>
       <c r="K40">
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2470,7 +2470,7 @@
         <v>43855</v>
       </c>
       <c r="K41">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2505,7 +2505,7 @@
         <v>43856</v>
       </c>
       <c r="K42">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2540,7 +2540,7 @@
         <v>43858</v>
       </c>
       <c r="K43">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2575,7 +2575,7 @@
         <v>43862</v>
       </c>
       <c r="K44">
-        <v>-4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2610,7 +2610,7 @@
         <v>43858</v>
       </c>
       <c r="K45">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2645,7 +2645,7 @@
         <v>43856</v>
       </c>
       <c r="K46">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2680,7 +2680,7 @@
         <v>43855</v>
       </c>
       <c r="K47">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2715,7 +2715,7 @@
         <v>43854</v>
       </c>
       <c r="K48">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2750,7 +2750,7 @@
         <v>43855</v>
       </c>
       <c r="K49">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2785,7 +2785,7 @@
         <v>43854</v>
       </c>
       <c r="K50">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2820,7 +2820,7 @@
         <v>43854</v>
       </c>
       <c r="K51">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2855,7 +2855,7 @@
         <v>43854</v>
       </c>
       <c r="K52">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2890,7 +2890,7 @@
         <v>43854</v>
       </c>
       <c r="K53">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2925,7 +2925,7 @@
         <v>43854</v>
       </c>
       <c r="K54">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2960,7 +2960,7 @@
         <v>43854</v>
       </c>
       <c r="K55">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2995,7 +2995,7 @@
         <v>43858</v>
       </c>
       <c r="K56">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3030,7 +3030,7 @@
         <v>43854</v>
       </c>
       <c r="K57">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3065,7 +3065,7 @@
         <v>43854</v>
       </c>
       <c r="K58">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3100,7 +3100,7 @@
         <v>43856</v>
       </c>
       <c r="K59">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3135,7 +3135,7 @@
         <v>43854</v>
       </c>
       <c r="K60">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3170,7 +3170,7 @@
         <v>43856</v>
       </c>
       <c r="K61">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3205,7 +3205,7 @@
         <v>43854</v>
       </c>
       <c r="K62">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3240,7 +3240,7 @@
         <v>43854</v>
       </c>
       <c r="K63">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3275,7 +3275,7 @@
         <v>43854</v>
       </c>
       <c r="K64">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3310,7 +3310,7 @@
         <v>43854</v>
       </c>
       <c r="K65">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -3345,7 +3345,7 @@
         <v>43854</v>
       </c>
       <c r="K66">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -3380,7 +3380,7 @@
         <v>43858</v>
       </c>
       <c r="K67">
-        <v>-9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -3415,7 +3415,7 @@
         <v>43855</v>
       </c>
       <c r="K68">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -3450,7 +3450,7 @@
         <v>43854</v>
       </c>
       <c r="K69">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3485,7 +3485,7 @@
         <v>43855</v>
       </c>
       <c r="K70">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3520,7 +3520,7 @@
         <v>43854</v>
       </c>
       <c r="K71">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -3555,7 +3555,7 @@
         <v>43855</v>
       </c>
       <c r="K72">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -3590,7 +3590,7 @@
         <v>43855</v>
       </c>
       <c r="K73">
-        <v>-12</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -3625,7 +3625,7 @@
         <v>43857</v>
       </c>
       <c r="K74">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -3660,7 +3660,7 @@
         <v>43854</v>
       </c>
       <c r="K75">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -3695,7 +3695,7 @@
         <v>43855</v>
       </c>
       <c r="K76">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -3730,7 +3730,7 @@
         <v>43854</v>
       </c>
       <c r="K77">
-        <v>-14</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -3765,7 +3765,7 @@
         <v>43854</v>
       </c>
       <c r="K78">
-        <v>-15</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -3800,7 +3800,7 @@
         <v>43854</v>
       </c>
       <c r="K79">
-        <v>-15</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -3835,7 +3835,7 @@
         <v>43855</v>
       </c>
       <c r="K80">
-        <v>-14</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -3870,7 +3870,7 @@
         <v>43854</v>
       </c>
       <c r="K81">
-        <v>-16</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -3905,7 +3905,7 @@
         <v>43856</v>
       </c>
       <c r="K82">
-        <v>-14</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3940,7 +3940,7 @@
         <v>43854</v>
       </c>
       <c r="K83">
-        <v>-17</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -3975,7 +3975,7 @@
         <v>43857</v>
       </c>
       <c r="K84">
-        <v>-14</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -4010,7 +4010,7 @@
         <v>43858</v>
       </c>
       <c r="K85">
-        <v>-16</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -4045,7 +4045,7 @@
         <v>43857</v>
       </c>
       <c r="K86">
-        <v>-17</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -4080,7 +4080,7 @@
         <v>43863</v>
       </c>
       <c r="K87">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -4115,7 +4115,7 @@
         <v>43855</v>
       </c>
       <c r="K88">
-        <v>-19</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4150,7 +4150,7 @@
         <v>43857</v>
       </c>
       <c r="K89">
-        <v>-17</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4185,7 +4185,7 @@
         <v>43855</v>
       </c>
       <c r="K90">
-        <v>-19</v>
+        <v>19</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4220,7 +4220,7 @@
         <v>43855</v>
       </c>
       <c r="K91">
-        <v>-19</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -4255,7 +4255,7 @@
         <v>43859</v>
       </c>
       <c r="K92">
-        <v>-15</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -4290,7 +4290,7 @@
         <v>43861</v>
       </c>
       <c r="K93">
-        <v>-13</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -4325,7 +4325,7 @@
         <v>43857</v>
       </c>
       <c r="K94">
-        <v>-17</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -4360,7 +4360,7 @@
         <v>43856</v>
       </c>
       <c r="K95">
-        <v>-18</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -4395,7 +4395,7 @@
         <v>43876</v>
       </c>
       <c r="K96">
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>